<commit_message>
stock updated for 06-09-2023
</commit_message>
<xml_diff>
--- a/TRADE_LIST.xlsx
+++ b/TRADE_LIST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji Lp\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji Lp\Documents\stock_updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E81FF31-52A8-403D-8977-0DDC5778C545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714F4D70-B9C1-49A6-97A7-32C6564D9CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{20DEF1ED-0919-437D-AD3F-D3C8E402565E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{20DEF1ED-0919-437D-AD3F-D3C8E402565E}"/>
   </bookViews>
   <sheets>
     <sheet name="AUGUST" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,6 +310,18 @@
     <font>
       <sz val="7"/>
       <color rgb="FF64B70B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF64B70B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFF54D4D"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -441,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -508,6 +520,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="34" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB095D83-4B35-4E3C-B8AA-78F6A8D5ABB6}">
   <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2240,45 +2254,11 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="G15:H15"/>
@@ -2295,11 +2275,45 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="U20:V20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2310,8 +2324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA03EABC-A62C-48C6-8225-3AF4DEACBF10}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2409,6 +2423,9 @@
       </c>
       <c r="D2" s="61">
         <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E2" s="66">
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -2430,6 +2447,9 @@
       <c r="D3" s="61">
         <v>3.5999999999999999E-3</v>
       </c>
+      <c r="E3" s="66">
+        <v>1.9400000000000001E-2</v>
+      </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="O3" s="10"/>
@@ -2450,6 +2470,9 @@
       <c r="D4" s="61">
         <v>1.15E-2</v>
       </c>
+      <c r="E4" s="67">
+        <v>-6.8999999999999999E-3</v>
+      </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="O4" s="10"/>
@@ -2470,6 +2493,9 @@
       <c r="D5" s="62">
         <v>-3.27E-2</v>
       </c>
+      <c r="E5" s="67">
+        <v>-8.2000000000000007E-3</v>
+      </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="O5" s="10"/>
@@ -2490,6 +2516,12 @@
       <c r="D6" s="62">
         <v>-2E-3</v>
       </c>
+      <c r="E6" s="67">
+        <v>-4.7000000000000002E-3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="O6" s="10"/>
@@ -2510,7 +2542,10 @@
       <c r="D7" s="62">
         <v>-1.8E-3</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="67">
+        <v>-8.0999999999999996E-3</v>
+      </c>
+      <c r="F7" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="10"/>
@@ -2533,8 +2568,8 @@
       <c r="D8" s="61">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="E8" t="s">
-        <v>24</v>
+      <c r="E8" s="66">
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -2556,7 +2591,10 @@
       <c r="D9" s="62">
         <v>-1.6899999999999998E-2</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="67">
+        <v>-2.4199999999999999E-2</v>
+      </c>
+      <c r="F9" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="10"/>
@@ -2579,6 +2617,9 @@
       <c r="D10" s="62">
         <v>-4.0000000000000002E-4</v>
       </c>
+      <c r="E10" s="67">
+        <v>-1.67E-2</v>
+      </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="O10" s="10"/>
@@ -2599,6 +2640,9 @@
       <c r="D11" s="62">
         <v>-1.8E-3</v>
       </c>
+      <c r="E11" s="67">
+        <v>-5.1000000000000004E-3</v>
+      </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="O11" s="10"/>
@@ -2619,6 +2663,9 @@
       <c r="D12" s="61">
         <v>2.1299999999999999E-2</v>
       </c>
+      <c r="E12" s="66">
+        <v>1.84E-2</v>
+      </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="O12" s="10"/>
@@ -2639,6 +2686,9 @@
       <c r="D13" s="62">
         <v>-5.1999999999999998E-3</v>
       </c>
+      <c r="E13" s="67">
+        <v>-6.4000000000000003E-3</v>
+      </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="O13" s="10"/>
@@ -2659,6 +2709,9 @@
       <c r="D14" s="61">
         <v>1.2800000000000001E-2</v>
       </c>
+      <c r="E14" s="66">
+        <v>9.9000000000000008E-3</v>
+      </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="O14" s="10"/>
@@ -2679,6 +2732,9 @@
       <c r="D15" s="61">
         <v>4.02E-2</v>
       </c>
+      <c r="E15" s="66">
+        <v>9.4999999999999998E-3</v>
+      </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="O15" s="10"/>
@@ -2699,6 +2755,9 @@
       <c r="D16" s="61">
         <v>1.5E-3</v>
       </c>
+      <c r="E16" s="67">
+        <v>-2.9999999999999997E-4</v>
+      </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="O16" s="10"/>
@@ -2719,7 +2778,10 @@
       <c r="D17" s="62">
         <v>-1.4200000000000001E-2</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="66">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F17" t="s">
         <v>24</v>
       </c>
       <c r="H17" s="10"/>
@@ -2742,6 +2804,9 @@
       <c r="D18" s="61">
         <v>1.2800000000000001E-2</v>
       </c>
+      <c r="E18" s="67">
+        <v>-1.2E-2</v>
+      </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="O18" s="10"/>
@@ -2762,6 +2827,9 @@
       <c r="D19" s="62">
         <v>-5.9999999999999995E-4</v>
       </c>
+      <c r="E19" s="67">
+        <v>-1.8599999999999998E-2</v>
+      </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="O19" s="10"/>
@@ -2782,6 +2850,9 @@
       <c r="D20" s="61">
         <v>5.6099999999999997E-2</v>
       </c>
+      <c r="E20" s="66">
+        <v>2.1899999999999999E-2</v>
+      </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="O20" s="10"/>
@@ -2802,6 +2873,9 @@
       <c r="D21" s="62">
         <v>-2.5000000000000001E-3</v>
       </c>
+      <c r="E21" s="66">
+        <v>1.1999999999999999E-3</v>
+      </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="O21" s="10"/>
@@ -2822,6 +2896,9 @@
       <c r="D22" s="62">
         <v>-9.2999999999999992E-3</v>
       </c>
+      <c r="E22" s="67">
+        <v>-7.0000000000000001E-3</v>
+      </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="O22" s="10"/>
@@ -2842,6 +2919,9 @@
       <c r="D23" s="61">
         <v>7.6E-3</v>
       </c>
+      <c r="E23" s="67">
+        <v>-1.6299999999999999E-2</v>
+      </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
       <c r="O23" s="10"/>
@@ -2861,6 +2941,9 @@
       </c>
       <c r="D24" s="62">
         <v>-8.3000000000000001E-3</v>
+      </c>
+      <c r="E24" s="67">
+        <v>-5.7999999999999996E-3</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
@@ -2883,17 +2966,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -2906,6 +2978,17 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated stock change percentage list so far
</commit_message>
<xml_diff>
--- a/TRADE_LIST.xlsx
+++ b/TRADE_LIST.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji Lp\Documents\stock_updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji Lp\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714F4D70-B9C1-49A6-97A7-32C6564D9CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF4AA57-A1FF-4A47-A6A5-D10E8B4F7DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{20DEF1ED-0919-437D-AD3F-D3C8E402565E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{20DEF1ED-0919-437D-AD3F-D3C8E402565E}"/>
   </bookViews>
   <sheets>
     <sheet name="AUGUST" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="25">
   <si>
     <t>MONEY'S</t>
   </si>
@@ -119,7 +119,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +327,12 @@
     </font>
     <font>
       <sz val="7"/>
+      <color rgb="FFF54D4D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
       <color rgb="FF64B70B"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -334,6 +340,12 @@
     <font>
       <sz val="7"/>
       <color rgb="FFF54D4D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF64B70B"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -453,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -517,11 +529,13 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="32" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="33" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="34" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="35" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB095D83-4B35-4E3C-B8AA-78F6A8D5ABB6}">
   <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z24" sqref="Z24"/>
+    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF9" sqref="AF9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,10 +975,10 @@
       <c r="F2" s="11">
         <v>-1.89E-2</v>
       </c>
-      <c r="G2" s="63" t="s">
+      <c r="G2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="65"/>
+      <c r="H2" s="67"/>
       <c r="I2" s="15">
         <v>-6.4000000000000003E-3</v>
       </c>
@@ -978,10 +992,10 @@
       <c r="M2" s="23">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="N2" s="63" t="s">
+      <c r="N2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="64"/>
+      <c r="O2" s="66"/>
       <c r="P2" s="41"/>
       <c r="Q2" s="34">
         <v>2.0999999999999999E-3</v>
@@ -993,10 +1007,10 @@
       <c r="T2" s="43">
         <v>-1.9599999999999999E-2</v>
       </c>
-      <c r="U2" s="63" t="s">
+      <c r="U2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="V2" s="64"/>
+      <c r="V2" s="66"/>
       <c r="W2" s="48">
         <v>1.6799999999999999E-2</v>
       </c>
@@ -1034,10 +1048,10 @@
       <c r="F3" s="11">
         <v>-1.8499999999999999E-2</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="G3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="65"/>
+      <c r="H3" s="67"/>
       <c r="I3" s="16">
         <v>1.4200000000000001E-2</v>
       </c>
@@ -1051,10 +1065,10 @@
       <c r="M3" s="23">
         <v>0</v>
       </c>
-      <c r="N3" s="63" t="s">
+      <c r="N3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="64"/>
+      <c r="O3" s="66"/>
       <c r="P3" s="35">
         <v>-3.2000000000000002E-3</v>
       </c>
@@ -1070,10 +1084,10 @@
       <c r="T3" s="43">
         <v>-7.6E-3</v>
       </c>
-      <c r="U3" s="63" t="s">
+      <c r="U3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="64"/>
+      <c r="V3" s="66"/>
       <c r="W3" s="49">
         <v>-1.9E-3</v>
       </c>
@@ -1113,10 +1127,10 @@
       <c r="F4" s="11">
         <v>-8.2000000000000007E-3</v>
       </c>
-      <c r="G4" s="63" t="s">
+      <c r="G4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="65"/>
+      <c r="H4" s="67"/>
       <c r="I4" s="15">
         <v>-1.9E-3</v>
       </c>
@@ -1130,10 +1144,10 @@
       <c r="M4" s="25">
         <v>-3.3E-3</v>
       </c>
-      <c r="N4" s="63" t="s">
+      <c r="N4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="64"/>
+      <c r="O4" s="66"/>
       <c r="P4" s="41"/>
       <c r="Q4" s="34">
         <v>1.34E-2</v>
@@ -1145,10 +1159,10 @@
       <c r="T4" s="42">
         <v>0</v>
       </c>
-      <c r="U4" s="63" t="s">
+      <c r="U4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="V4" s="64"/>
+      <c r="V4" s="66"/>
       <c r="W4" s="48">
         <v>2.3800000000000002E-2</v>
       </c>
@@ -1186,10 +1200,10 @@
       <c r="F5" s="12">
         <v>0.1152</v>
       </c>
-      <c r="G5" s="63" t="s">
+      <c r="G5" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="65"/>
+      <c r="H5" s="67"/>
       <c r="I5" s="16">
         <v>2.9399999999999999E-2</v>
       </c>
@@ -1203,10 +1217,10 @@
       <c r="M5" s="25">
         <v>-3.6600000000000001E-2</v>
       </c>
-      <c r="N5" s="63" t="s">
+      <c r="N5" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="64"/>
+      <c r="O5" s="66"/>
       <c r="P5" s="41"/>
       <c r="Q5" s="34">
         <v>1.7100000000000001E-2</v>
@@ -1218,10 +1232,10 @@
       <c r="T5" s="43">
         <v>-2.6499999999999999E-2</v>
       </c>
-      <c r="U5" s="63" t="s">
+      <c r="U5" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="V5" s="64"/>
+      <c r="V5" s="66"/>
       <c r="W5" s="48">
         <v>4.4499999999999998E-2</v>
       </c>
@@ -1259,10 +1273,10 @@
       <c r="F6" s="11">
         <v>-3.2300000000000002E-2</v>
       </c>
-      <c r="G6" s="63" t="s">
+      <c r="G6" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="65"/>
+      <c r="H6" s="67"/>
       <c r="I6" s="15">
         <v>-2.8799999999999999E-2</v>
       </c>
@@ -1276,10 +1290,10 @@
       <c r="M6" s="23">
         <v>1.03E-2</v>
       </c>
-      <c r="N6" s="63" t="s">
+      <c r="N6" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="64"/>
+      <c r="O6" s="66"/>
       <c r="P6" s="41"/>
       <c r="Q6" s="34">
         <v>1.78E-2</v>
@@ -1291,10 +1305,10 @@
       <c r="T6" s="43">
         <v>-8.3000000000000001E-3</v>
       </c>
-      <c r="U6" s="63" t="s">
+      <c r="U6" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="V6" s="64"/>
+      <c r="V6" s="66"/>
       <c r="W6" s="48">
         <v>1.1900000000000001E-2</v>
       </c>
@@ -1332,10 +1346,10 @@
       <c r="F7" s="13">
         <v>-2.5600000000000001E-2</v>
       </c>
-      <c r="G7" s="63" t="s">
+      <c r="G7" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="65"/>
+      <c r="H7" s="67"/>
       <c r="I7" s="17">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -1349,10 +1363,10 @@
       <c r="M7" s="27">
         <v>-3.5999999999999999E-3</v>
       </c>
-      <c r="N7" s="63" t="s">
+      <c r="N7" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="64"/>
+      <c r="O7" s="66"/>
       <c r="P7" s="37"/>
       <c r="Q7" s="36">
         <v>5.0000000000000001E-3</v>
@@ -1364,10 +1378,10 @@
       <c r="T7" s="46">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="U7" s="63" t="s">
+      <c r="U7" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="V7" s="64"/>
+      <c r="V7" s="66"/>
       <c r="W7" s="49">
         <v>-1.4500000000000001E-2</v>
       </c>
@@ -1405,10 +1419,10 @@
       <c r="F8" s="12">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="G8" s="63" t="s">
+      <c r="G8" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="65"/>
+      <c r="H8" s="67"/>
       <c r="I8" s="16">
         <v>1.3299999999999999E-2</v>
       </c>
@@ -1422,10 +1436,10 @@
       <c r="M8" s="25">
         <v>-1.7999999999999999E-2</v>
       </c>
-      <c r="N8" s="63" t="s">
+      <c r="N8" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="O8" s="64"/>
+      <c r="O8" s="66"/>
       <c r="P8" s="41"/>
       <c r="Q8" s="35">
         <v>-1.26E-2</v>
@@ -1437,10 +1451,10 @@
       <c r="T8" s="43">
         <v>-1.6199999999999999E-2</v>
       </c>
-      <c r="U8" s="63" t="s">
+      <c r="U8" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="V8" s="64"/>
+      <c r="V8" s="66"/>
       <c r="W8" s="49">
         <v>-2.7300000000000001E-2</v>
       </c>
@@ -1480,10 +1494,10 @@
       <c r="F9" s="12">
         <v>0.04</v>
       </c>
-      <c r="G9" s="63" t="s">
+      <c r="G9" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="65"/>
+      <c r="H9" s="67"/>
       <c r="I9" s="16">
         <v>3.5000000000000001E-3</v>
       </c>
@@ -1497,10 +1511,10 @@
       <c r="M9" s="23">
         <v>1.49E-2</v>
       </c>
-      <c r="N9" s="63" t="s">
+      <c r="N9" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="64"/>
+      <c r="O9" s="66"/>
       <c r="P9" s="41"/>
       <c r="Q9" s="35">
         <v>-1.3299999999999999E-2</v>
@@ -1512,10 +1526,10 @@
       <c r="T9" s="42">
         <v>2.06E-2</v>
       </c>
-      <c r="U9" s="63" t="s">
+      <c r="U9" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="V9" s="64"/>
+      <c r="V9" s="66"/>
       <c r="W9" s="49">
         <v>-1.2E-2</v>
       </c>
@@ -1553,10 +1567,10 @@
       <c r="F10" s="12">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="G10" s="63" t="s">
+      <c r="G10" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="65"/>
+      <c r="H10" s="67"/>
       <c r="I10" s="15">
         <v>-1.7899999999999999E-2</v>
       </c>
@@ -1570,10 +1584,10 @@
       <c r="M10" s="25">
         <v>-2.2000000000000001E-3</v>
       </c>
-      <c r="N10" s="63" t="s">
+      <c r="N10" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="64"/>
+      <c r="O10" s="66"/>
       <c r="P10" s="41"/>
       <c r="Q10" s="34">
         <v>5.5999999999999999E-3</v>
@@ -1585,10 +1599,10 @@
       <c r="T10" s="43">
         <v>-1.14E-2</v>
       </c>
-      <c r="U10" s="63" t="s">
+      <c r="U10" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="V10" s="64"/>
+      <c r="V10" s="66"/>
       <c r="W10" s="48">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -1626,10 +1640,10 @@
       <c r="F11" s="11">
         <v>-1.2699999999999999E-2</v>
       </c>
-      <c r="G11" s="63" t="s">
+      <c r="G11" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="65"/>
+      <c r="H11" s="67"/>
       <c r="I11" s="15">
         <v>-4.0000000000000002E-4</v>
       </c>
@@ -1643,10 +1657,10 @@
       <c r="M11" s="25">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="N11" s="63" t="s">
+      <c r="N11" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="64"/>
+      <c r="O11" s="66"/>
       <c r="P11" s="41"/>
       <c r="Q11" s="35">
         <v>-4.5999999999999999E-3</v>
@@ -1658,10 +1672,10 @@
       <c r="T11" s="43">
         <v>-8.0000000000000002E-3</v>
       </c>
-      <c r="U11" s="63" t="s">
+      <c r="U11" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="V11" s="64"/>
+      <c r="V11" s="66"/>
       <c r="W11" s="49">
         <v>-4.1999999999999997E-3</v>
       </c>
@@ -1699,10 +1713,10 @@
       <c r="F12" s="12">
         <v>3.7199999999999997E-2</v>
       </c>
-      <c r="G12" s="63" t="s">
+      <c r="G12" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="65"/>
+      <c r="H12" s="67"/>
       <c r="I12" s="16">
         <v>3.4700000000000002E-2</v>
       </c>
@@ -1716,10 +1730,10 @@
       <c r="M12" s="23">
         <v>1.78E-2</v>
       </c>
-      <c r="N12" s="63" t="s">
+      <c r="N12" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="O12" s="64"/>
+      <c r="O12" s="66"/>
       <c r="P12" s="41"/>
       <c r="Q12" s="35">
         <v>-5.2200000000000003E-2</v>
@@ -1731,10 +1745,10 @@
       <c r="T12" s="42">
         <v>1.15E-2</v>
       </c>
-      <c r="U12" s="63" t="s">
+      <c r="U12" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="V12" s="64"/>
+      <c r="V12" s="66"/>
       <c r="W12" s="48">
         <v>2.5499999999999998E-2</v>
       </c>
@@ -1772,10 +1786,10 @@
       <c r="F13" s="11">
         <v>-1.35E-2</v>
       </c>
-      <c r="G13" s="63" t="s">
+      <c r="G13" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="65"/>
+      <c r="H13" s="67"/>
       <c r="I13" s="16">
         <v>2.3E-3</v>
       </c>
@@ -1789,10 +1803,10 @@
       <c r="M13" s="25">
         <v>-1.4E-2</v>
       </c>
-      <c r="N13" s="63" t="s">
+      <c r="N13" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="O13" s="64"/>
+      <c r="O13" s="66"/>
       <c r="P13" s="41"/>
       <c r="Q13" s="34">
         <v>6.0000000000000001E-3</v>
@@ -1804,10 +1818,10 @@
       <c r="T13" s="43">
         <v>-7.3000000000000001E-3</v>
       </c>
-      <c r="U13" s="63" t="s">
+      <c r="U13" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="V13" s="64"/>
+      <c r="V13" s="66"/>
       <c r="W13" s="49">
         <v>-4.3E-3</v>
       </c>
@@ -1845,10 +1859,10 @@
       <c r="F14" s="13">
         <v>-6.7999999999999996E-3</v>
       </c>
-      <c r="G14" s="63" t="s">
+      <c r="G14" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="65"/>
+      <c r="H14" s="67"/>
       <c r="I14" s="16">
         <v>4.0000000000000002E-4</v>
       </c>
@@ -1862,10 +1876,10 @@
       <c r="M14" s="29">
         <v>1.5E-3</v>
       </c>
-      <c r="N14" s="63" t="s">
+      <c r="N14" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="O14" s="64"/>
+      <c r="O14" s="66"/>
       <c r="P14" s="47">
         <v>1.34</v>
       </c>
@@ -1879,10 +1893,10 @@
       <c r="T14" s="43">
         <v>-1.67E-2</v>
       </c>
-      <c r="U14" s="63" t="s">
+      <c r="U14" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="V14" s="64"/>
+      <c r="V14" s="66"/>
       <c r="W14" s="49">
         <v>-4.4999999999999997E-3</v>
       </c>
@@ -1910,10 +1924,10 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="14"/>
-      <c r="G15" s="63" t="s">
+      <c r="G15" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="65"/>
+      <c r="H15" s="67"/>
       <c r="I15" s="18"/>
       <c r="J15" s="10"/>
       <c r="K15" s="19">
@@ -1925,10 +1939,10 @@
       <c r="M15" s="23">
         <v>8.6E-3</v>
       </c>
-      <c r="N15" s="63" t="s">
+      <c r="N15" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="O15" s="64"/>
+      <c r="O15" s="66"/>
       <c r="P15" s="41"/>
       <c r="Q15" s="34">
         <v>5.9999999999999995E-4</v>
@@ -1940,10 +1954,10 @@
       <c r="T15" s="43">
         <v>-1.4E-3</v>
       </c>
-      <c r="U15" s="63" t="s">
+      <c r="U15" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="V15" s="64"/>
+      <c r="V15" s="66"/>
       <c r="W15" s="48">
         <v>8.0000000000000004E-4</v>
       </c>
@@ -1963,17 +1977,17 @@
       <c r="AC15" s="10"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="N16" s="63" t="s">
+      <c r="N16" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="O16" s="64"/>
+      <c r="O16" s="66"/>
       <c r="T16" s="43">
         <v>-2.9899999999999999E-2</v>
       </c>
-      <c r="U16" s="63" t="s">
+      <c r="U16" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="V16" s="64"/>
+      <c r="V16" s="66"/>
       <c r="W16" s="48">
         <v>1.46E-2</v>
       </c>
@@ -1993,17 +2007,17 @@
       <c r="AC16" s="10"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="N17" s="63" t="s">
+      <c r="N17" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="O17" s="64"/>
+      <c r="O17" s="66"/>
       <c r="T17" s="43">
         <v>-2.1700000000000001E-2</v>
       </c>
-      <c r="U17" s="63" t="s">
+      <c r="U17" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="V17" s="64"/>
+      <c r="V17" s="66"/>
       <c r="W17" s="48">
         <v>2.7000000000000001E-3</v>
       </c>
@@ -2025,17 +2039,17 @@
       <c r="AC17" s="10"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="N18" s="63" t="s">
+      <c r="N18" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="O18" s="64"/>
+      <c r="O18" s="66"/>
       <c r="T18" s="43">
         <v>-4.3E-3</v>
       </c>
-      <c r="U18" s="63" t="s">
+      <c r="U18" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="V18" s="64"/>
+      <c r="V18" s="66"/>
       <c r="W18" s="48">
         <v>2.4199999999999999E-2</v>
       </c>
@@ -2055,17 +2069,17 @@
       <c r="AC18" s="10"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="N19" s="63" t="s">
+      <c r="N19" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="O19" s="64"/>
+      <c r="O19" s="66"/>
       <c r="T19" s="43">
         <v>-8.3999999999999995E-3</v>
       </c>
-      <c r="U19" s="63" t="s">
+      <c r="U19" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="V19" s="64"/>
+      <c r="V19" s="66"/>
       <c r="W19" s="48">
         <v>3.8999999999999998E-3</v>
       </c>
@@ -2085,17 +2099,17 @@
       <c r="AC19" s="10"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="N20" s="63" t="s">
+      <c r="N20" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="O20" s="64"/>
+      <c r="O20" s="66"/>
       <c r="T20" s="43">
         <v>-3.0999999999999999E-3</v>
       </c>
-      <c r="U20" s="63" t="s">
+      <c r="U20" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="V20" s="64"/>
+      <c r="V20" s="66"/>
       <c r="W20" s="49">
         <v>-8.0000000000000004E-4</v>
       </c>
@@ -2117,17 +2131,17 @@
       <c r="AC20" s="10"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="N21" s="63" t="s">
+      <c r="N21" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="O21" s="64"/>
+      <c r="O21" s="66"/>
       <c r="T21" s="43">
         <v>-5.7999999999999996E-3</v>
       </c>
-      <c r="U21" s="63" t="s">
+      <c r="U21" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="V21" s="64"/>
+      <c r="V21" s="66"/>
       <c r="W21" s="48">
         <v>6.7999999999999996E-3</v>
       </c>
@@ -2147,17 +2161,17 @@
       <c r="AC21" s="10"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="N22" s="63" t="s">
+      <c r="N22" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="O22" s="64"/>
+      <c r="O22" s="66"/>
       <c r="T22" s="43">
         <v>-1.26E-2</v>
       </c>
-      <c r="U22" s="63" t="s">
+      <c r="U22" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="V22" s="64"/>
+      <c r="V22" s="66"/>
       <c r="W22" s="49">
         <v>-2.5000000000000001E-3</v>
       </c>
@@ -2177,17 +2191,17 @@
       <c r="AC22" s="10"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="N23" s="63" t="s">
+      <c r="N23" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="O23" s="64"/>
+      <c r="O23" s="66"/>
       <c r="T23" s="43">
         <v>-3.8E-3</v>
       </c>
-      <c r="U23" s="63" t="s">
+      <c r="U23" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="V23" s="64"/>
+      <c r="V23" s="66"/>
       <c r="W23" s="49">
         <v>-8.0000000000000004E-4</v>
       </c>
@@ -2208,17 +2222,17 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="N24" s="63" t="s">
+      <c r="N24" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="O24" s="64"/>
+      <c r="O24" s="66"/>
       <c r="T24" s="43">
         <v>-2.7099999999999999E-2</v>
       </c>
-      <c r="U24" s="63" t="s">
+      <c r="U24" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="V24" s="64"/>
+      <c r="V24" s="66"/>
       <c r="W24" s="49">
         <v>-1.11E-2</v>
       </c>
@@ -2254,11 +2268,45 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="G15:H15"/>
@@ -2275,45 +2323,11 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2324,8 +2338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA03EABC-A62C-48C6-8225-3AF4DEACBF10}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2414,18 +2428,21 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="66"/>
       <c r="C2" s="58">
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="D2" s="61">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="E2" s="66">
-        <v>8.3999999999999995E-3</v>
+      <c r="E2" s="64">
+        <v>-6.7000000000000002E-3</v>
+      </c>
+      <c r="F2" s="69">
+        <v>-4.4999999999999997E-3</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -2437,18 +2454,21 @@
       <c r="AC2" s="10"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="64"/>
+      <c r="B3" s="66"/>
       <c r="C3" s="58">
         <v>1.12E-2</v>
       </c>
       <c r="D3" s="61">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="E3" s="66">
-        <v>1.9400000000000001E-2</v>
+      <c r="E3" s="64">
+        <v>-3.8E-3</v>
+      </c>
+      <c r="F3" s="68">
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -2460,18 +2480,21 @@
       <c r="AC3" s="10"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="64"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="59">
         <v>-5.1999999999999998E-3</v>
       </c>
       <c r="D4" s="61">
         <v>1.15E-2</v>
       </c>
-      <c r="E4" s="67">
-        <v>-6.8999999999999999E-3</v>
+      <c r="E4" s="63">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="F4" s="68">
+        <v>1.72E-2</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -2483,18 +2506,21 @@
       <c r="AC4" s="10"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="64"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="58">
         <v>2.18E-2</v>
       </c>
       <c r="D5" s="62">
         <v>-3.27E-2</v>
       </c>
-      <c r="E5" s="67">
-        <v>-8.2000000000000007E-3</v>
+      <c r="E5" s="63">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="F5" s="68">
+        <v>1.6899999999999998E-2</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
@@ -2506,21 +2532,21 @@
       <c r="AC5" s="10"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="59">
         <v>-6.9999999999999999E-4</v>
       </c>
       <c r="D6" s="62">
         <v>-2E-3</v>
       </c>
-      <c r="E6" s="67">
-        <v>-4.7000000000000002E-3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
+      <c r="E6" s="63">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="F6" s="69">
+        <v>-3.5499999999999997E-2</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -2532,21 +2558,21 @@
       <c r="AC6" s="10"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="59">
         <v>-1.9E-3</v>
       </c>
       <c r="D7" s="62">
         <v>-1.8E-3</v>
       </c>
-      <c r="E7" s="67">
-        <v>-8.0999999999999996E-3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
+      <c r="E7" s="64">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="F7" s="68">
+        <v>1.8E-3</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -2558,18 +2584,21 @@
       <c r="AC7" s="10"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="64"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="59">
         <v>-2.52E-2</v>
       </c>
       <c r="D8" s="61">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="E8" s="66">
-        <v>6.4000000000000003E-3</v>
+      <c r="E8" s="63">
+        <v>4.9200000000000001E-2</v>
+      </c>
+      <c r="F8" s="68">
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -2581,21 +2610,21 @@
       <c r="AC8" s="10"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="64"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="59">
         <v>-9.4000000000000004E-3</v>
       </c>
       <c r="D9" s="62">
         <v>-1.6899999999999998E-2</v>
       </c>
-      <c r="E9" s="67">
-        <v>-2.4199999999999999E-2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
+      <c r="E9" s="64">
+        <v>-1.7100000000000001E-2</v>
+      </c>
+      <c r="F9" s="69">
+        <v>-2.9999999999999997E-4</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -2607,18 +2636,21 @@
       <c r="AC9" s="10"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="64"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="58">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="D10" s="62">
         <v>-4.0000000000000002E-4</v>
       </c>
-      <c r="E10" s="67">
-        <v>-1.67E-2</v>
+      <c r="E10" s="63">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="F10" s="69">
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -2630,18 +2662,21 @@
       <c r="AC10" s="10"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="64"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="58">
         <v>1.7399999999999999E-2</v>
       </c>
       <c r="D11" s="62">
         <v>-1.8E-3</v>
       </c>
-      <c r="E11" s="67">
-        <v>-5.1000000000000004E-3</v>
+      <c r="E11" s="63">
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="F11" s="69">
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -2653,18 +2688,21 @@
       <c r="AC11" s="10"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="64"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="58">
         <v>3.3700000000000001E-2</v>
       </c>
       <c r="D12" s="61">
         <v>2.1299999999999999E-2</v>
       </c>
-      <c r="E12" s="66">
-        <v>1.84E-2</v>
+      <c r="E12" s="64">
+        <v>-2.5000000000000001E-3</v>
+      </c>
+      <c r="F12" s="68">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -2676,18 +2714,21 @@
       <c r="AC12" s="10"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="64"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="58">
         <v>4.2599999999999999E-2</v>
       </c>
       <c r="D13" s="62">
         <v>-5.1999999999999998E-3</v>
       </c>
-      <c r="E13" s="67">
-        <v>-6.4000000000000003E-3</v>
+      <c r="E13" s="63">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="F13" s="69">
+        <v>-6.6E-3</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -2699,18 +2740,21 @@
       <c r="AC13" s="10"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A14" s="63" t="s">
+      <c r="A14" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="64"/>
+      <c r="B14" s="66"/>
       <c r="C14" s="59">
         <v>-8.0000000000000002E-3</v>
       </c>
       <c r="D14" s="61">
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="E14" s="66">
-        <v>9.9000000000000008E-3</v>
+      <c r="E14" s="64">
+        <v>-3.5000000000000001E-3</v>
+      </c>
+      <c r="F14" s="69">
+        <v>-7.3000000000000001E-3</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -2722,18 +2766,21 @@
       <c r="AC14" s="10"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="64"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="59">
         <v>-1.1000000000000001E-3</v>
       </c>
       <c r="D15" s="61">
         <v>4.02E-2</v>
       </c>
-      <c r="E15" s="66">
-        <v>9.4999999999999998E-3</v>
+      <c r="E15" s="63">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="F15" s="69">
+        <v>-7.6E-3</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -2745,18 +2792,21 @@
       <c r="AC15" s="10"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="64"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="58">
         <v>8.6999999999999994E-3</v>
       </c>
       <c r="D16" s="61">
         <v>1.5E-3</v>
       </c>
-      <c r="E16" s="67">
-        <v>-2.9999999999999997E-4</v>
+      <c r="E16" s="63">
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="F16" s="69">
+        <v>-4.4999999999999997E-3</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -2768,21 +2818,21 @@
       <c r="AC16" s="10"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="64"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="58">
         <v>1.4500000000000001E-2</v>
       </c>
       <c r="D17" s="62">
         <v>-1.4200000000000001E-2</v>
       </c>
-      <c r="E17" s="66">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="F17" t="s">
-        <v>24</v>
+      <c r="E17" s="63">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="F17" s="69">
+        <v>-5.5999999999999999E-3</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
@@ -2794,18 +2844,21 @@
       <c r="AC17" s="10"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="64"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="58">
         <v>1.7399999999999999E-2</v>
       </c>
       <c r="D18" s="61">
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="E18" s="67">
-        <v>-1.2E-2</v>
+      <c r="E18" s="64">
+        <v>-3.5999999999999999E-3</v>
+      </c>
+      <c r="F18" s="69">
+        <v>-8.0000000000000004E-4</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -2817,18 +2870,21 @@
       <c r="AC18" s="10"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="64"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="58">
         <v>3.4200000000000001E-2</v>
       </c>
       <c r="D19" s="62">
         <v>-5.9999999999999995E-4</v>
       </c>
-      <c r="E19" s="67">
-        <v>-1.8599999999999998E-2</v>
+      <c r="E19" s="63">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="F19" s="69">
+        <v>-6.0000000000000001E-3</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -2840,18 +2896,21 @@
       <c r="AC19" s="10"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="64"/>
+      <c r="B20" s="66"/>
       <c r="C20" s="58">
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="D20" s="61">
         <v>5.6099999999999997E-2</v>
       </c>
-      <c r="E20" s="66">
-        <v>2.1899999999999999E-2</v>
+      <c r="E20" s="64">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+      <c r="F20" s="69">
+        <v>-1.15E-2</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -2863,18 +2922,21 @@
       <c r="AC20" s="10"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="64"/>
+      <c r="B21" s="66"/>
       <c r="C21" s="58">
         <v>5.3E-3</v>
       </c>
       <c r="D21" s="62">
         <v>-2.5000000000000001E-3</v>
       </c>
-      <c r="E21" s="66">
-        <v>1.1999999999999999E-3</v>
+      <c r="E21" s="63">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="F21" s="68">
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
@@ -2886,18 +2948,21 @@
       <c r="AC21" s="10"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="64"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="58">
         <v>4.6600000000000003E-2</v>
       </c>
       <c r="D22" s="62">
         <v>-9.2999999999999992E-3</v>
       </c>
-      <c r="E22" s="67">
-        <v>-7.0000000000000001E-3</v>
+      <c r="E22" s="63">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="F22" s="68">
+        <v>7.7999999999999996E-3</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
@@ -2909,18 +2974,21 @@
       <c r="AC22" s="10"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A23" s="63" t="s">
+      <c r="A23" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="64"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="58">
         <v>5.4100000000000002E-2</v>
       </c>
       <c r="D23" s="61">
         <v>7.6E-3</v>
       </c>
-      <c r="E23" s="67">
-        <v>-1.6299999999999999E-2</v>
+      <c r="E23" s="64">
+        <v>-1.89E-2</v>
+      </c>
+      <c r="F23" s="69">
+        <v>-4.7000000000000002E-3</v>
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
@@ -2932,18 +3000,21 @@
       <c r="AC23" s="10"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A24" s="63" t="s">
+      <c r="A24" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="64"/>
+      <c r="B24" s="66"/>
       <c r="C24" s="58">
         <v>4.0899999999999999E-2</v>
       </c>
       <c r="D24" s="62">
         <v>-8.3000000000000001E-3</v>
       </c>
-      <c r="E24" s="67">
-        <v>-5.7999999999999996E-3</v>
+      <c r="E24" s="63">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="F24" s="69">
+        <v>-6.1999999999999998E-3</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
@@ -2966,6 +3037,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -2978,17 +3060,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>